<commit_message>
Rewrote cleaning chesstempo manual tactical puzzles
</commit_message>
<xml_diff>
--- a/data/input/manual_puzzles.xlsx
+++ b/data/input/manual_puzzles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="1474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="1565">
   <si>
     <t>969.4</t>
   </si>
@@ -4446,6 +4446,279 @@
   </si>
   <si>
     <t>1439.9 (+3.1)</t>
+  </si>
+  <si>
+    <t>1358.0</t>
+  </si>
+  <si>
+    <t>1449.0 (-4.4)</t>
+  </si>
+  <si>
+    <t>1322.4</t>
+  </si>
+  <si>
+    <t>1453.4 (+2.3)</t>
+  </si>
+  <si>
+    <t>1536.7</t>
+  </si>
+  <si>
+    <t>1451.1 (+4.4)</t>
+  </si>
+  <si>
+    <t>1369.0</t>
+  </si>
+  <si>
+    <t>1446.7 (+2.7)</t>
+  </si>
+  <si>
+    <t>1320.3</t>
+  </si>
+  <si>
+    <t>1444.0 (+2.3)</t>
+  </si>
+  <si>
+    <t>1357.7</t>
+  </si>
+  <si>
+    <t>1441.7 (+2.7)</t>
+  </si>
+  <si>
+    <t>1439.0 (+1.5)</t>
+  </si>
+  <si>
+    <t>1476.8</t>
+  </si>
+  <si>
+    <t>1437.5 (-3.1)</t>
+  </si>
+  <si>
+    <t>1268.5</t>
+  </si>
+  <si>
+    <t>1440.6 (-5.1)</t>
+  </si>
+  <si>
+    <t>1066.6</t>
+  </si>
+  <si>
+    <t>1445.8 (+0.7)</t>
+  </si>
+  <si>
+    <t>1301.6</t>
+  </si>
+  <si>
+    <t>1445.0 (-4.9)</t>
+  </si>
+  <si>
+    <t>1449.9 (-4.8)</t>
+  </si>
+  <si>
+    <t>1452.6</t>
+  </si>
+  <si>
+    <t>1454.8 (-3.5)</t>
+  </si>
+  <si>
+    <t>1458.3 (+2.8)</t>
+  </si>
+  <si>
+    <t>1157.0</t>
+  </si>
+  <si>
+    <t>1455.5 (+1.1)</t>
+  </si>
+  <si>
+    <t>1454.4 (+1.7)</t>
+  </si>
+  <si>
+    <t>1385.0</t>
+  </si>
+  <si>
+    <t>1452.7 (+2.8)</t>
+  </si>
+  <si>
+    <t>1257.0</t>
+  </si>
+  <si>
+    <t>1449.9 (+1.7)</t>
+  </si>
+  <si>
+    <t>1448.2 (+1.8)</t>
+  </si>
+  <si>
+    <t>1274.0</t>
+  </si>
+  <si>
+    <t>1446.4 (+1.9)</t>
+  </si>
+  <si>
+    <t>1250.4</t>
+  </si>
+  <si>
+    <t>1444.4 (+1.7)</t>
+  </si>
+  <si>
+    <t>1370.4</t>
+  </si>
+  <si>
+    <t>1442.7 (-4.2)</t>
+  </si>
+  <si>
+    <t>1324.8</t>
+  </si>
+  <si>
+    <t>1446.9 (-4.7)</t>
+  </si>
+  <si>
+    <t>1488.1</t>
+  </si>
+  <si>
+    <t>1451.7 (+3.9)</t>
+  </si>
+  <si>
+    <t>1248.5</t>
+  </si>
+  <si>
+    <t>1447.8 (-5.3)</t>
+  </si>
+  <si>
+    <t>1354.6</t>
+  </si>
+  <si>
+    <t>1453.1 (+2.6)</t>
+  </si>
+  <si>
+    <t>1450.6 (-4.6)</t>
+  </si>
+  <si>
+    <t>1439.3</t>
+  </si>
+  <si>
+    <t>1455.2 (-3.7)</t>
+  </si>
+  <si>
+    <t>1458.9 (+2.1)</t>
+  </si>
+  <si>
+    <t>1408.1</t>
+  </si>
+  <si>
+    <t>1456.8 (-4.0)</t>
+  </si>
+  <si>
+    <t>1460.8 (+1.3)</t>
+  </si>
+  <si>
+    <t>1398.0</t>
+  </si>
+  <si>
+    <t>1459.5 (-4.1)</t>
+  </si>
+  <si>
+    <t>1332.9</t>
+  </si>
+  <si>
+    <t>1463.6 (+2.3)</t>
+  </si>
+  <si>
+    <t>1320.2</t>
+  </si>
+  <si>
+    <t>1461.3 (+2.2)</t>
+  </si>
+  <si>
+    <t>1489.4</t>
+  </si>
+  <si>
+    <t>1459.2 (+3.8)</t>
+  </si>
+  <si>
+    <t>1474.0</t>
+  </si>
+  <si>
+    <t>1455.3 (+3.7)</t>
+  </si>
+  <si>
+    <t>1471.7</t>
+  </si>
+  <si>
+    <t>1451.6 (-3.3)</t>
+  </si>
+  <si>
+    <t>1387.2</t>
+  </si>
+  <si>
+    <t>1454.9 (+2.8)</t>
+  </si>
+  <si>
+    <t>1452.1 (-3.7)</t>
+  </si>
+  <si>
+    <t>1457.5 (+1.4)</t>
+  </si>
+  <si>
+    <t>1461.8</t>
+  </si>
+  <si>
+    <t>1456.0 (-3.5)</t>
+  </si>
+  <si>
+    <t>1459.5 (+2.3)</t>
+  </si>
+  <si>
+    <t>1345.6</t>
+  </si>
+  <si>
+    <t>1457.2 (+2.4)</t>
+  </si>
+  <si>
+    <t>1555.0</t>
+  </si>
+  <si>
+    <t>1454.7 (-2.5)</t>
+  </si>
+  <si>
+    <t>1215.3</t>
+  </si>
+  <si>
+    <t>1457.3 (+1.4)</t>
+  </si>
+  <si>
+    <t>1479.6</t>
+  </si>
+  <si>
+    <t>1455.9 (+3.8)</t>
+  </si>
+  <si>
+    <t>1351.6</t>
+  </si>
+  <si>
+    <t>1452.1 (+2.5)</t>
+  </si>
+  <si>
+    <t>1391.4</t>
+  </si>
+  <si>
+    <t>1449.6 (-4.1)</t>
+  </si>
+  <si>
+    <t>1475.5</t>
+  </si>
+  <si>
+    <t>1453.7 (+3.7)</t>
+  </si>
+  <si>
+    <t>1432.0</t>
+  </si>
+  <si>
+    <t>1450.0 (-3.7)</t>
+  </si>
+  <si>
+    <t>1574.1</t>
+  </si>
+  <si>
+    <t>1453.7 (+4.7)</t>
   </si>
 </sst>
 </file>
@@ -4767,15 +5040,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I775"/>
+  <dimension ref="A1:I826"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A742" workbookViewId="0">
-      <selection activeCell="J758" sqref="J758"/>
+    <sheetView tabSelected="1" topLeftCell="A799" workbookViewId="0">
+      <selection activeCell="A815" sqref="A815:I826"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -27253,6 +27527,1485 @@
         <v>1473</v>
       </c>
     </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A776">
+        <v>1</v>
+      </c>
+      <c r="B776" s="1">
+        <v>42766.635509259257</v>
+      </c>
+      <c r="C776">
+        <v>44527</v>
+      </c>
+      <c r="D776" t="s">
+        <v>1474</v>
+      </c>
+      <c r="E776" t="s">
+        <v>1</v>
+      </c>
+      <c r="F776" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="G776" s="2">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="H776" s="2">
+        <v>0</v>
+      </c>
+      <c r="I776" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A777">
+        <v>2</v>
+      </c>
+      <c r="B777" s="1">
+        <v>42766.631956018522</v>
+      </c>
+      <c r="C777">
+        <v>152707</v>
+      </c>
+      <c r="D777" t="s">
+        <v>1476</v>
+      </c>
+      <c r="E777" t="s">
+        <v>1</v>
+      </c>
+      <c r="F777" s="2">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="G777" s="2">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="H777" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I777" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="778" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A778">
+        <v>3</v>
+      </c>
+      <c r="B778" s="1">
+        <v>42766.631643518522</v>
+      </c>
+      <c r="C778">
+        <v>64486</v>
+      </c>
+      <c r="D778" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E778" t="s">
+        <v>1</v>
+      </c>
+      <c r="F778" s="2">
+        <v>0.10625</v>
+      </c>
+      <c r="G778" s="2">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="H778" s="2">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="I778" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A779">
+        <v>4</v>
+      </c>
+      <c r="B779" s="1">
+        <v>42766.630104166667</v>
+      </c>
+      <c r="C779">
+        <v>102920</v>
+      </c>
+      <c r="D779" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E779" t="s">
+        <v>1</v>
+      </c>
+      <c r="F779" s="2">
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="G779" s="2">
+        <v>0.17986111111111111</v>
+      </c>
+      <c r="H779" s="2">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="I779" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A780">
+        <v>5</v>
+      </c>
+      <c r="B780" s="1">
+        <v>42766.627060185187</v>
+      </c>
+      <c r="C780">
+        <v>51180</v>
+      </c>
+      <c r="D780" t="s">
+        <v>1482</v>
+      </c>
+      <c r="E780" t="s">
+        <v>1</v>
+      </c>
+      <c r="F780" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G780" s="3">
+        <v>1.3951388888888889</v>
+      </c>
+      <c r="H780" s="2">
+        <v>0</v>
+      </c>
+      <c r="I780" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A781">
+        <v>6</v>
+      </c>
+      <c r="B781" s="1">
+        <v>42766.603715277779</v>
+      </c>
+      <c r="C781">
+        <v>76084</v>
+      </c>
+      <c r="D781" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E781" t="s">
+        <v>1</v>
+      </c>
+      <c r="F781" s="2">
+        <v>9.6527777777777768E-2</v>
+      </c>
+      <c r="G781" s="2">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="H781" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="I781" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A782">
+        <v>7</v>
+      </c>
+      <c r="B782" s="1">
+        <v>42766.602789351855</v>
+      </c>
+      <c r="C782">
+        <v>71693</v>
+      </c>
+      <c r="D782" t="s">
+        <v>368</v>
+      </c>
+      <c r="E782" t="s">
+        <v>1</v>
+      </c>
+      <c r="F782" s="2">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G782" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="H782" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="I782" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="783" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A783">
+        <v>8</v>
+      </c>
+      <c r="B783" s="1">
+        <v>42766.601712962962</v>
+      </c>
+      <c r="C783">
+        <v>72501</v>
+      </c>
+      <c r="D783" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E783" t="s">
+        <v>1</v>
+      </c>
+      <c r="F783" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="G783" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H783" s="2">
+        <v>0</v>
+      </c>
+      <c r="I783" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="784" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A784">
+        <v>9</v>
+      </c>
+      <c r="B784" s="1">
+        <v>42766.597418981481</v>
+      </c>
+      <c r="C784">
+        <v>60047</v>
+      </c>
+      <c r="D784" t="s">
+        <v>1489</v>
+      </c>
+      <c r="E784" t="s">
+        <v>1</v>
+      </c>
+      <c r="F784" s="2">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="G784" s="2">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="H784" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I784" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="785" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A785">
+        <v>10</v>
+      </c>
+      <c r="B785" s="1">
+        <v>42766.597129629627</v>
+      </c>
+      <c r="C785">
+        <v>105110</v>
+      </c>
+      <c r="D785" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E785" t="s">
+        <v>1</v>
+      </c>
+      <c r="F785" s="2">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="G785" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H785" s="2">
+        <v>0</v>
+      </c>
+      <c r="I785" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="786" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A786">
+        <v>11</v>
+      </c>
+      <c r="B786" s="1">
+        <v>42766.596435185187</v>
+      </c>
+      <c r="C786">
+        <v>46011</v>
+      </c>
+      <c r="D786" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E786" t="s">
+        <v>1</v>
+      </c>
+      <c r="F786" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="G786" s="2">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H786" s="2">
+        <v>0</v>
+      </c>
+      <c r="I786" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="787" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A787">
+        <v>12</v>
+      </c>
+      <c r="B787" s="1">
+        <v>42766.595763888887</v>
+      </c>
+      <c r="C787">
+        <v>89463</v>
+      </c>
+      <c r="D787" t="s">
+        <v>890</v>
+      </c>
+      <c r="E787" t="s">
+        <v>1</v>
+      </c>
+      <c r="F787" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G787" s="2">
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="H787" s="2">
+        <v>0</v>
+      </c>
+      <c r="I787" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="788" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A788">
+        <v>13</v>
+      </c>
+      <c r="B788" s="1">
+        <v>42766.591122685182</v>
+      </c>
+      <c r="C788">
+        <v>73684</v>
+      </c>
+      <c r="D788" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E788" t="s">
+        <v>1</v>
+      </c>
+      <c r="F788" s="2">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="G788" s="2">
+        <v>0.15416666666666667</v>
+      </c>
+      <c r="H788" s="2">
+        <v>0</v>
+      </c>
+      <c r="I788" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="789" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A789">
+        <v>14</v>
+      </c>
+      <c r="B789" s="1">
+        <v>42766.588518518518</v>
+      </c>
+      <c r="C789">
+        <v>149669</v>
+      </c>
+      <c r="D789" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E789" t="s">
+        <v>1</v>
+      </c>
+      <c r="F789" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G789" s="2">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="H789" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I789" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="790" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A790">
+        <v>15</v>
+      </c>
+      <c r="B790" s="1">
+        <v>42766.586388888885</v>
+      </c>
+      <c r="C790">
+        <v>60063</v>
+      </c>
+      <c r="D790" t="s">
+        <v>1499</v>
+      </c>
+      <c r="E790" t="s">
+        <v>1</v>
+      </c>
+      <c r="F790" s="2">
+        <v>3.9583333333333331E-2</v>
+      </c>
+      <c r="G790" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H790" s="2">
+        <v>0</v>
+      </c>
+      <c r="I790" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="791" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A791">
+        <v>16</v>
+      </c>
+      <c r="B791" s="1">
+        <v>42766.585972222223</v>
+      </c>
+      <c r="C791">
+        <v>169677</v>
+      </c>
+      <c r="D791" t="s">
+        <v>276</v>
+      </c>
+      <c r="E791" t="s">
+        <v>1</v>
+      </c>
+      <c r="F791" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G791" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="H791" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I791" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="792" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A792">
+        <v>17</v>
+      </c>
+      <c r="B792" s="1">
+        <v>42766.585219907407</v>
+      </c>
+      <c r="C792">
+        <v>44354</v>
+      </c>
+      <c r="D792" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E792" t="s">
+        <v>1</v>
+      </c>
+      <c r="F792" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G792" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="H792" s="2">
+        <v>0</v>
+      </c>
+      <c r="I792" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="793" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A793">
+        <v>18</v>
+      </c>
+      <c r="B793" s="1">
+        <v>42766.58494212963</v>
+      </c>
+      <c r="C793">
+        <v>61405</v>
+      </c>
+      <c r="D793" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E793" t="s">
+        <v>1</v>
+      </c>
+      <c r="F793" s="2">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="G793" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="H793" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I793" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="794" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A794">
+        <v>19</v>
+      </c>
+      <c r="B794" s="1">
+        <v>42766.58357638889</v>
+      </c>
+      <c r="C794">
+        <v>97239</v>
+      </c>
+      <c r="D794" t="s">
+        <v>931</v>
+      </c>
+      <c r="E794" t="s">
+        <v>1</v>
+      </c>
+      <c r="F794" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="G794" s="2">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="H794" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I794" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="795" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A795">
+        <v>20</v>
+      </c>
+      <c r="B795" s="1">
+        <v>42766.583298611113</v>
+      </c>
+      <c r="C795">
+        <v>43693</v>
+      </c>
+      <c r="D795" t="s">
+        <v>1507</v>
+      </c>
+      <c r="E795" t="s">
+        <v>1</v>
+      </c>
+      <c r="F795" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="G795" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H795" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I795" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="796" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A796">
+        <v>21</v>
+      </c>
+      <c r="B796" s="1">
+        <v>42766.58289351852</v>
+      </c>
+      <c r="C796">
+        <v>158716</v>
+      </c>
+      <c r="D796" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E796" t="s">
+        <v>1</v>
+      </c>
+      <c r="F796" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G796" s="2">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="H796" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I796" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="797" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A797">
+        <v>22</v>
+      </c>
+      <c r="B797" s="1">
+        <v>42766.582361111112</v>
+      </c>
+      <c r="C797">
+        <v>167676</v>
+      </c>
+      <c r="D797" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E797" t="s">
+        <v>1</v>
+      </c>
+      <c r="F797" s="2">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="G797" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H797" s="2">
+        <v>0</v>
+      </c>
+      <c r="I797" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="798" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A798">
+        <v>23</v>
+      </c>
+      <c r="B798" s="1">
+        <v>42766.581678240742</v>
+      </c>
+      <c r="C798">
+        <v>93998</v>
+      </c>
+      <c r="D798" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E798" t="s">
+        <v>1</v>
+      </c>
+      <c r="F798" s="2">
+        <v>0.10833333333333334</v>
+      </c>
+      <c r="G798" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H798" s="2">
+        <v>0</v>
+      </c>
+      <c r="I798" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="799" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A799">
+        <v>24</v>
+      </c>
+      <c r="B799" s="1">
+        <v>42766.572962962964</v>
+      </c>
+      <c r="C799">
+        <v>64935</v>
+      </c>
+      <c r="D799" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E799" t="s">
+        <v>1</v>
+      </c>
+      <c r="F799" s="2">
+        <v>0.10555555555555556</v>
+      </c>
+      <c r="G799" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="H799" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I799" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="800" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A800">
+        <v>25</v>
+      </c>
+      <c r="B800" s="1">
+        <v>42766.572280092594</v>
+      </c>
+      <c r="C800">
+        <v>23888</v>
+      </c>
+      <c r="D800" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E800" t="s">
+        <v>1</v>
+      </c>
+      <c r="F800" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="G800" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H800" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I800" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="801" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A801">
+        <v>26</v>
+      </c>
+      <c r="B801" s="1">
+        <v>42766.571944444448</v>
+      </c>
+      <c r="C801">
+        <v>626</v>
+      </c>
+      <c r="D801" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E801" t="s">
+        <v>1</v>
+      </c>
+      <c r="F801" s="2">
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="G801" s="2">
+        <v>0.1763888888888889</v>
+      </c>
+      <c r="H801" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I801" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="802" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A802">
+        <v>27</v>
+      </c>
+      <c r="B802" s="1">
+        <v>42766.56890046296</v>
+      </c>
+      <c r="C802">
+        <v>48354</v>
+      </c>
+      <c r="D802" t="s">
+        <v>794</v>
+      </c>
+      <c r="E802" t="s">
+        <v>1</v>
+      </c>
+      <c r="F802" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="G802" s="2">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H802" s="2">
+        <v>0</v>
+      </c>
+      <c r="I802" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="803" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A803">
+        <v>28</v>
+      </c>
+      <c r="B803" s="1">
+        <v>42766.568055555559</v>
+      </c>
+      <c r="C803">
+        <v>148365</v>
+      </c>
+      <c r="D803" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E803" t="s">
+        <v>1</v>
+      </c>
+      <c r="F803" s="2">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="G803" s="2">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="H803" s="2">
+        <v>0</v>
+      </c>
+      <c r="I803" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="804" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A804">
+        <v>29</v>
+      </c>
+      <c r="B804" s="1">
+        <v>42766.567442129628</v>
+      </c>
+      <c r="C804">
+        <v>166370</v>
+      </c>
+      <c r="D804" t="s">
+        <v>961</v>
+      </c>
+      <c r="E804" t="s">
+        <v>1</v>
+      </c>
+      <c r="F804" s="2">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="G804" s="2">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H804" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I804" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="805" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A805">
+        <v>30</v>
+      </c>
+      <c r="B805" s="1">
+        <v>42766.56689814815</v>
+      </c>
+      <c r="C805">
+        <v>169424</v>
+      </c>
+      <c r="D805" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E805" t="s">
+        <v>1</v>
+      </c>
+      <c r="F805" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="G805" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="H805" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="I805" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="806" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A806">
+        <v>31</v>
+      </c>
+      <c r="B806" s="1">
+        <v>42766.566053240742</v>
+      </c>
+      <c r="C806">
+        <v>153919</v>
+      </c>
+      <c r="D806" t="s">
+        <v>699</v>
+      </c>
+      <c r="E806" t="s">
+        <v>1</v>
+      </c>
+      <c r="F806" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="G806" s="2">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H806" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="I806" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="807" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A807">
+        <v>32</v>
+      </c>
+      <c r="B807" s="1">
+        <v>42766.512430555558</v>
+      </c>
+      <c r="C807">
+        <v>177046</v>
+      </c>
+      <c r="D807" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E807" t="s">
+        <v>1</v>
+      </c>
+      <c r="F807" s="2">
+        <v>0.21805555555555556</v>
+      </c>
+      <c r="G807" s="2">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="H807" s="2">
+        <v>0</v>
+      </c>
+      <c r="I807" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="808" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A808">
+        <v>33</v>
+      </c>
+      <c r="B808" s="1">
+        <v>42766.508333333331</v>
+      </c>
+      <c r="C808">
+        <v>77616</v>
+      </c>
+      <c r="D808" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E808" t="s">
+        <v>1</v>
+      </c>
+      <c r="F808" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G808" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H808" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I808" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="809" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A809">
+        <v>34</v>
+      </c>
+      <c r="B809" s="1">
+        <v>42766.496076388888</v>
+      </c>
+      <c r="C809">
+        <v>60678</v>
+      </c>
+      <c r="D809" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E809" t="s">
+        <v>1</v>
+      </c>
+      <c r="F809" s="2">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="G809" s="2">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="H809" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I809" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="810" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A810">
+        <v>35</v>
+      </c>
+      <c r="B810" s="1">
+        <v>42766.495358796295</v>
+      </c>
+      <c r="C810">
+        <v>153101</v>
+      </c>
+      <c r="D810" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E810" t="s">
+        <v>1</v>
+      </c>
+      <c r="F810" s="2">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="G810" s="2">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="H810" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="I810" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="811" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A811">
+        <v>36</v>
+      </c>
+      <c r="B811" s="1">
+        <v>42766.494016203702</v>
+      </c>
+      <c r="C811">
+        <v>141745</v>
+      </c>
+      <c r="D811" t="s">
+        <v>1536</v>
+      </c>
+      <c r="E811" t="s">
+        <v>1</v>
+      </c>
+      <c r="F811" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="G811" s="2">
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="H811" s="2">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="I811" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="812" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A812">
+        <v>37</v>
+      </c>
+      <c r="B812" s="1">
+        <v>42766.491446759261</v>
+      </c>
+      <c r="C812">
+        <v>59608</v>
+      </c>
+      <c r="D812" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E812" t="s">
+        <v>1</v>
+      </c>
+      <c r="F812" s="2">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="G812" s="2">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="H812" s="2">
+        <v>0</v>
+      </c>
+      <c r="I812" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="813" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A813">
+        <v>38</v>
+      </c>
+      <c r="B813" s="1">
+        <v>42766.487638888888</v>
+      </c>
+      <c r="C813">
+        <v>97636</v>
+      </c>
+      <c r="D813" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E813" t="s">
+        <v>1</v>
+      </c>
+      <c r="F813" s="2">
+        <v>8.2638888888888887E-2</v>
+      </c>
+      <c r="G813" s="2">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="H813" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I813" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="814" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A814">
+        <v>39</v>
+      </c>
+      <c r="B814" s="1">
+        <v>42766.486215277779</v>
+      </c>
+      <c r="C814">
+        <v>177474</v>
+      </c>
+      <c r="D814" t="s">
+        <v>953</v>
+      </c>
+      <c r="E814" t="s">
+        <v>1</v>
+      </c>
+      <c r="F814" s="2">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="G814" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="H814" s="2">
+        <v>0</v>
+      </c>
+      <c r="I814" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="815" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A815">
+        <v>1</v>
+      </c>
+      <c r="B815" s="1">
+        <v>42766.789039351854</v>
+      </c>
+      <c r="C815">
+        <v>56152</v>
+      </c>
+      <c r="D815" t="s">
+        <v>804</v>
+      </c>
+      <c r="E815" t="s">
+        <v>1</v>
+      </c>
+      <c r="F815" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G815" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H815" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I815" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="816" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A816">
+        <v>2</v>
+      </c>
+      <c r="B816" s="1">
+        <v>42766.788263888891</v>
+      </c>
+      <c r="C816">
+        <v>155879</v>
+      </c>
+      <c r="D816" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E816" t="s">
+        <v>1</v>
+      </c>
+      <c r="F816" s="2">
+        <v>0.13263888888888889</v>
+      </c>
+      <c r="G816" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="H816" s="2">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="I816" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="817" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A817">
+        <v>3</v>
+      </c>
+      <c r="B817" s="1">
+        <v>42766.787465277775</v>
+      </c>
+      <c r="C817">
+        <v>176348</v>
+      </c>
+      <c r="D817" t="s">
+        <v>754</v>
+      </c>
+      <c r="E817" t="s">
+        <v>1</v>
+      </c>
+      <c r="F817" s="2">
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="G817" s="2">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="H817" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I817" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="818" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A818">
+        <v>4</v>
+      </c>
+      <c r="B818" s="1">
+        <v>42766.782696759263</v>
+      </c>
+      <c r="C818">
+        <v>47622</v>
+      </c>
+      <c r="D818" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E818" t="s">
+        <v>1</v>
+      </c>
+      <c r="F818" s="2">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="G818" s="2">
+        <v>0.10972222222222222</v>
+      </c>
+      <c r="H818" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I818" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="819" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A819">
+        <v>5</v>
+      </c>
+      <c r="B819" s="1">
+        <v>42766.780115740738</v>
+      </c>
+      <c r="C819">
+        <v>57090</v>
+      </c>
+      <c r="D819" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E819" t="s">
+        <v>1</v>
+      </c>
+      <c r="F819" s="2">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="G819" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="H819" s="2">
+        <v>0</v>
+      </c>
+      <c r="I819" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="820" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A820">
+        <v>6</v>
+      </c>
+      <c r="B820" s="1">
+        <v>42766.779270833336</v>
+      </c>
+      <c r="C820">
+        <v>63674</v>
+      </c>
+      <c r="D820" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E820" t="s">
+        <v>1</v>
+      </c>
+      <c r="F820" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G820" s="2">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="H820" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I820" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="821" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A821">
+        <v>7</v>
+      </c>
+      <c r="B821" s="1">
+        <v>42766.777777777781</v>
+      </c>
+      <c r="C821">
+        <v>21770</v>
+      </c>
+      <c r="D821" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E821" t="s">
+        <v>1</v>
+      </c>
+      <c r="F821" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G821" s="2">
+        <v>0.19722222222222222</v>
+      </c>
+      <c r="H821" s="2">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="I821" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="822" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A822">
+        <v>8</v>
+      </c>
+      <c r="B822" s="1">
+        <v>42766.774247685185</v>
+      </c>
+      <c r="C822">
+        <v>177321</v>
+      </c>
+      <c r="D822" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E822" t="s">
+        <v>1</v>
+      </c>
+      <c r="F822" s="2">
+        <v>0.12152777777777778</v>
+      </c>
+      <c r="G822" s="2">
+        <v>0.28680555555555554</v>
+      </c>
+      <c r="H822" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="I822" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="823" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A823">
+        <v>9</v>
+      </c>
+      <c r="B823" s="1">
+        <v>42766.768888888888</v>
+      </c>
+      <c r="C823">
+        <v>63713</v>
+      </c>
+      <c r="D823" t="s">
+        <v>1557</v>
+      </c>
+      <c r="E823" t="s">
+        <v>1</v>
+      </c>
+      <c r="F823" s="2">
+        <v>0.1013888888888889</v>
+      </c>
+      <c r="G823" s="2">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="H823" s="2">
+        <v>0</v>
+      </c>
+      <c r="I823" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="824" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A824">
+        <v>10</v>
+      </c>
+      <c r="B824" s="1">
+        <v>42766.761701388888</v>
+      </c>
+      <c r="C824">
+        <v>141295</v>
+      </c>
+      <c r="D824" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E824" t="s">
+        <v>1</v>
+      </c>
+      <c r="F824" s="2">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="G824" s="2">
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="H824" s="2">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="I824" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="825" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A825">
+        <v>11</v>
+      </c>
+      <c r="B825" s="1">
+        <v>42766.759085648147</v>
+      </c>
+      <c r="C825">
+        <v>105499</v>
+      </c>
+      <c r="D825" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E825" t="s">
+        <v>1</v>
+      </c>
+      <c r="F825" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G825" s="2">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="H825" s="2">
+        <v>0</v>
+      </c>
+      <c r="I825" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="826" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A826">
+        <v>12</v>
+      </c>
+      <c r="B826" s="1">
+        <v>42766.758634259262</v>
+      </c>
+      <c r="C826">
+        <v>164890</v>
+      </c>
+      <c r="D826" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E826" t="s">
+        <v>1</v>
+      </c>
+      <c r="F826" s="2">
+        <v>0.19375000000000001</v>
+      </c>
+      <c r="G826" s="4">
+        <v>0.12293981481481481</v>
+      </c>
+      <c r="H826" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I826" t="s">
+        <v>1564</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>